<commit_message>
Updated examples based on the lastest CDS-on-FHIR profiles.
</commit_message>
<xml_diff>
--- a/Docs/KnowledgeModule_Metadata_Mappings.xlsx
+++ b/Docs/KnowledgeModule_Metadata_Mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryn\Documents\Src\HL7\Specifications\CDS FHIR Profiles\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryn\Documents\Src\SS\CQFIG\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -466,9 +466,6 @@
     <t>FHIR Representation (as basic profile)</t>
   </si>
   <si>
-    <t>KnowledgeModule.moduleIdentifier + version</t>
-  </si>
-  <si>
     <t>KnowledgeModule.version</t>
   </si>
   <si>
@@ -539,6 +536,12 @@
   </si>
   <si>
     <t>KnowledgeModule.contributor</t>
+  </si>
+  <si>
+    <t>Resource.id</t>
+  </si>
+  <si>
+    <t>Basic.identifier (use=primary)</t>
   </si>
 </sst>
 </file>
@@ -1074,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,7 +1121,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1135,7 +1138,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>9</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1152,7 +1155,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1169,7 +1172,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1186,7 +1189,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1248,7 +1251,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -1316,7 +1319,7 @@
         <v>44</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1331,7 +1334,7 @@
         <v>46</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1346,7 +1349,7 @@
         <v>48</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1361,7 +1364,7 @@
         <v>50</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1376,7 +1379,7 @@
         <v>53</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1391,7 +1394,7 @@
         <v>56</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1406,7 +1409,7 @@
         <v>58</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1421,7 +1424,7 @@
         <v>60</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1466,7 +1469,7 @@
         <v>67</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1481,7 +1484,7 @@
         <v>69</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1496,7 +1499,7 @@
         <v>71</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1511,7 +1514,7 @@
         <v>73</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1526,7 +1529,7 @@
         <v>75</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1541,7 +1544,7 @@
         <v>78</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1556,7 +1559,7 @@
         <v>80</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1584,7 +1587,7 @@
         <v>84</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1599,7 +1602,7 @@
         <v>87</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -1614,7 +1617,7 @@
         <v>90</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -1629,7 +1632,7 @@
         <v>93</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -1644,7 +1647,7 @@
         <v>96</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1659,7 +1662,7 @@
         <v>98</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1689,7 +1692,7 @@
         <v>103</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1704,7 +1707,7 @@
         <v>105</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1719,7 +1722,7 @@
         <v>105</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1734,7 +1737,7 @@
         <v>110</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>